<commit_message>
fixing problems and last changes
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol-Plami.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol-Plami.xlsx
@@ -683,7 +683,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +773,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="12">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" s="6"/>
     </row>

</xml_diff>

<commit_message>
changes in the evaluation protokol
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol-Plami.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol-Plami.xlsx
@@ -685,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -776,7 +776,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="12">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6"/>
     </row>

</xml_diff>